<commit_message>
Fixing Iran FC Team Icons
</commit_message>
<xml_diff>
--- a/Documantation/Final/Teams.xlsx
+++ b/Documantation/Final/Teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Project\Hamed Soleimani\Handy Football\Documantation\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A692EE-0229-4889-A877-697ED353E380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE64BED3-420D-4F68-955A-9017E46B7017}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="552" windowWidth="11496" windowHeight="11304" xr2:uid="{ECF06A1F-CD2B-45BD-8D37-BFC9939645AD}"/>
   </bookViews>
@@ -234,12 +234,6 @@
     <t>Saipa</t>
   </si>
   <si>
-    <t>Rah Ahan Tehran</t>
-  </si>
-  <si>
-    <t>راه آهن تهران</t>
-  </si>
-  <si>
     <t>Zob Ahan</t>
   </si>
   <si>
@@ -258,48 +252,6 @@
     <t>استقلال خوزستان</t>
   </si>
   <si>
-    <t>Gostaresh Foolad</t>
-  </si>
-  <si>
-    <t>گسترش فولاد</t>
-  </si>
-  <si>
-    <t>Malavan Anzali</t>
-  </si>
-  <si>
-    <t>ملوان انزلی</t>
-  </si>
-  <si>
-    <t>Paykan Qazvin</t>
-  </si>
-  <si>
-    <t>پیکان قزوین</t>
-  </si>
-  <si>
-    <t>Naft Talaieh</t>
-  </si>
-  <si>
-    <t>نفت طلائیه</t>
-  </si>
-  <si>
-    <t>Padideh Shandiz</t>
-  </si>
-  <si>
-    <t>پدیده شیراز</t>
-  </si>
-  <si>
-    <t>Sabaye Qom</t>
-  </si>
-  <si>
-    <t>صبای قم</t>
-  </si>
-  <si>
-    <t>Aboumoslem Khorasan</t>
-  </si>
-  <si>
-    <t>ابومسلم خراسان</t>
-  </si>
-  <si>
     <t>Arsenal</t>
   </si>
   <si>
@@ -397,6 +349,54 @@
   </si>
   <si>
     <t>Numbers</t>
+  </si>
+  <si>
+    <t>Padideh Shahr Khodro</t>
+  </si>
+  <si>
+    <t>پدیده شهر خودرو</t>
+  </si>
+  <si>
+    <t>Sanat Naft Abadan</t>
+  </si>
+  <si>
+    <t>صنعت نفت آبادان</t>
+  </si>
+  <si>
+    <t>Nassagi Mazandaran</t>
+  </si>
+  <si>
+    <t>نساجی مازندران</t>
+  </si>
+  <si>
+    <t>Paykan</t>
+  </si>
+  <si>
+    <t>پیکان</t>
+  </si>
+  <si>
+    <t>Pars Jonobi Jam</t>
+  </si>
+  <si>
+    <t>Mashin Saazi Tabriz</t>
+  </si>
+  <si>
+    <t>Naft Masjed Soleiman</t>
+  </si>
+  <si>
+    <t>Sepid Rood Rasht</t>
+  </si>
+  <si>
+    <t>پارس  جنوبی جم</t>
+  </si>
+  <si>
+    <t>ماشین سازی تبریز</t>
+  </si>
+  <si>
+    <t>نفت مسجد سلیمان</t>
+  </si>
+  <si>
+    <t>سپید رود رشت</t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3753AAEB-6318-494D-9F15-E9F1EFFD60D3}">
   <dimension ref="S1:U63"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="O43" workbookViewId="0">
-      <selection activeCell="S63" sqref="S63"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="O33" workbookViewId="0">
+      <selection activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="U1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="19:21" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
     </row>
     <row r="31" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S31" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="T31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="U31">
         <v>28</v>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="32" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T32" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="U32">
         <v>29</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="33" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="T33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="U33">
         <v>30</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="34" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S34" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="T34" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="U34">
         <v>31</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="35" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S35" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="T35" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="U35">
         <v>32</v>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="37" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="T37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="U37">
         <v>34</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="38" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="T38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="U38">
         <v>35</v>
@@ -1174,10 +1174,10 @@
     </row>
     <row r="39" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S39" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="T39" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="U39">
         <v>36</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="40" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S40" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="T40" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="U40">
         <v>37</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="41" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S41" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="T41" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="U41">
         <v>38</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="42" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S42" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="T42" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="U42">
         <v>39</v>
@@ -1218,10 +1218,10 @@
     </row>
     <row r="43" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S43" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="T43" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="U43">
         <v>40</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="44" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S44" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="T44" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="U44">
         <v>41</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="45" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S45" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="T45" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="U45">
         <v>42</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="46" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S46" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="T46" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="U46">
         <v>43</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="48" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S48" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="T48" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="U48">
         <v>44</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="49" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S49" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="T49" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="U49">
         <v>45</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="50" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S50" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="T50" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="U50">
         <v>46</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="51" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S51" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="T51" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="U51">
         <v>47</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="52" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S52" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="T52" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="U52">
         <v>48</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="53" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S53" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="T53" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="U53">
         <v>49</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="54" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S54" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="T54" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="U54">
         <v>50</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="55" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S55" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="T55" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="U55">
         <v>51</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="56" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S56" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="T56" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="U56">
         <v>52</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="57" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S57" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="T57" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="U57">
         <v>53</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="58" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S58" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="T58" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="U58">
         <v>54</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="59" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S59" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="T59" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="U59">
         <v>55</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="60" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S60" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="T60" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="U60">
         <v>56</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="61" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S61" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="T61" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="U61">
         <v>57</v>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="62" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S62" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="T62" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="U62">
         <v>58</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="63" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S63" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="T63" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="U63">
         <v>59</v>

</xml_diff>

<commit_message>
Fixing National Team And Team Manager ID
</commit_message>
<xml_diff>
--- a/Documantation/Final/Teams.xlsx
+++ b/Documantation/Final/Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Project\Hamed Soleimani\Handy Football\Documantation\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE64BED3-420D-4F68-955A-9017E46B7017}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC83FF31-E373-408B-8A03-CA7197E01913}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="552" windowWidth="11496" windowHeight="11304" xr2:uid="{ECF06A1F-CD2B-45BD-8D37-BFC9939645AD}"/>
+    <workbookView xWindow="5928" yWindow="480" windowWidth="11496" windowHeight="11304" xr2:uid="{ECF06A1F-CD2B-45BD-8D37-BFC9939645AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Iran FC</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>سپید رود رشت</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -748,22 +754,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3753AAEB-6318-494D-9F15-E9F1EFFD60D3}">
-  <dimension ref="S1:U63"/>
+  <dimension ref="P1:U63"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="O33" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N42" workbookViewId="0">
+      <selection activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="17" max="17" width="4.5" customWidth="1"/>
+    <col min="15" max="15" width="7.3984375" customWidth="1"/>
+    <col min="16" max="16" width="8.796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.19921875" customWidth="1"/>
     <col min="18" max="18" width="12.796875" customWidth="1"/>
     <col min="19" max="19" width="17.8984375" customWidth="1"/>
     <col min="20" max="20" width="20.5" customWidth="1"/>
     <col min="21" max="21" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
+        <v>124</v>
+      </c>
       <c r="T1" t="s">
         <v>2</v>
       </c>
@@ -771,7 +785,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
+      </c>
       <c r="S2" t="s">
         <v>31</v>
       </c>
@@ -782,7 +802,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>9</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
       <c r="S3" t="s">
         <v>32</v>
       </c>
@@ -793,7 +819,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
       <c r="S4" t="s">
         <v>33</v>
       </c>
@@ -804,7 +836,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
       <c r="S5" t="s">
         <v>34</v>
       </c>
@@ -815,7 +853,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
       <c r="S6" t="s">
         <v>35</v>
       </c>
@@ -826,7 +870,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>10</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
       <c r="S7" t="s">
         <v>36</v>
       </c>
@@ -837,7 +887,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>9</v>
+      </c>
       <c r="S8" t="s">
         <v>37</v>
       </c>
@@ -848,7 +904,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
       <c r="S9" t="s">
         <v>38</v>
       </c>
@@ -859,7 +921,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
       <c r="S10" t="s">
         <v>39</v>
       </c>
@@ -870,7 +938,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
       <c r="S11" t="s">
         <v>40</v>
       </c>
@@ -881,7 +955,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
       <c r="S12" t="s">
         <v>41</v>
       </c>
@@ -892,7 +972,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
       <c r="S13" t="s">
         <v>42</v>
       </c>
@@ -903,7 +989,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>9</v>
+      </c>
       <c r="S14" t="s">
         <v>43</v>
       </c>
@@ -914,7 +1006,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>9</v>
+      </c>
       <c r="S15" t="s">
         <v>44</v>
       </c>
@@ -925,7 +1023,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
       <c r="S16" t="s">
         <v>45</v>
       </c>
@@ -936,7 +1040,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>7</v>
+      </c>
       <c r="S17" t="s">
         <v>46</v>
       </c>
@@ -947,7 +1057,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>8</v>
+      </c>
       <c r="S18" t="s">
         <v>47</v>
       </c>
@@ -958,7 +1074,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>7</v>
+      </c>
       <c r="S19" t="s">
         <v>48</v>
       </c>
@@ -969,7 +1091,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
       <c r="S20" t="s">
         <v>49</v>
       </c>
@@ -980,7 +1108,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>8</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
+      </c>
       <c r="S21" t="s">
         <v>50</v>
       </c>
@@ -991,7 +1125,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>6</v>
+      </c>
+      <c r="R22">
+        <v>5</v>
+      </c>
       <c r="S22" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1142,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>3</v>
+      </c>
+      <c r="R23">
+        <v>8</v>
+      </c>
       <c r="S23" t="s">
         <v>52</v>
       </c>
@@ -1013,7 +1159,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>9</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
       <c r="S24" t="s">
         <v>53</v>
       </c>
@@ -1024,7 +1176,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>6</v>
+      </c>
+      <c r="R25">
+        <v>3</v>
+      </c>
       <c r="S25" t="s">
         <v>54</v>
       </c>
@@ -1035,7 +1193,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>7</v>
+      </c>
+      <c r="R26">
+        <v>5</v>
+      </c>
       <c r="S26" t="s">
         <v>55</v>
       </c>
@@ -1046,7 +1210,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>9</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
       <c r="S27" t="s">
         <v>56</v>
       </c>
@@ -1057,7 +1227,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>3</v>
+      </c>
+      <c r="R28">
+        <v>9</v>
+      </c>
       <c r="S28" t="s">
         <v>57</v>
       </c>
@@ -1068,7 +1244,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>10</v>
+      </c>
+      <c r="R29">
+        <v>3</v>
+      </c>
       <c r="S29" t="s">
         <v>58</v>
       </c>
@@ -1079,12 +1261,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="17:21" x14ac:dyDescent="0.25">
       <c r="T30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>4</v>
+      </c>
+      <c r="R31">
+        <v>9</v>
+      </c>
       <c r="S31" t="s">
         <v>62</v>
       </c>
@@ -1095,7 +1283,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>5</v>
+      </c>
+      <c r="R32">
+        <v>8</v>
+      </c>
       <c r="S32" t="s">
         <v>64</v>
       </c>
@@ -1106,7 +1300,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="R33">
+        <v>9</v>
+      </c>
       <c r="S33" t="s">
         <v>60</v>
       </c>
@@ -1117,7 +1317,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>4</v>
+      </c>
+      <c r="R34">
+        <v>8</v>
+      </c>
       <c r="S34" t="s">
         <v>109</v>
       </c>
@@ -1128,7 +1334,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>5</v>
+      </c>
+      <c r="R35">
+        <v>7</v>
+      </c>
       <c r="S35" t="s">
         <v>72</v>
       </c>
@@ -1139,7 +1351,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>4</v>
+      </c>
+      <c r="R36">
+        <v>8</v>
+      </c>
       <c r="S36" t="s">
         <v>70</v>
       </c>
@@ -1150,7 +1368,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>6</v>
+      </c>
+      <c r="R37">
+        <v>7</v>
+      </c>
       <c r="S37" t="s">
         <v>67</v>
       </c>
@@ -1161,7 +1385,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>4</v>
+      </c>
+      <c r="R38">
+        <v>6</v>
+      </c>
       <c r="S38" t="s">
         <v>66</v>
       </c>
@@ -1172,7 +1402,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>6</v>
+      </c>
+      <c r="R39">
+        <v>6</v>
+      </c>
       <c r="S39" t="s">
         <v>111</v>
       </c>
@@ -1183,7 +1419,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>6</v>
+      </c>
+      <c r="R40">
+        <v>5</v>
+      </c>
       <c r="S40" t="s">
         <v>113</v>
       </c>
@@ -1194,7 +1436,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>4</v>
+      </c>
+      <c r="R41">
+        <v>8</v>
+      </c>
       <c r="S41" t="s">
         <v>115</v>
       </c>
@@ -1205,7 +1453,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>7</v>
+      </c>
+      <c r="R42">
+        <v>4</v>
+      </c>
       <c r="S42" t="s">
         <v>120</v>
       </c>
@@ -1216,7 +1470,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>6</v>
+      </c>
+      <c r="R43">
+        <v>3</v>
+      </c>
       <c r="S43" t="s">
         <v>121</v>
       </c>
@@ -1227,7 +1487,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>8</v>
+      </c>
+      <c r="R44">
+        <v>2</v>
+      </c>
       <c r="S44" t="s">
         <v>122</v>
       </c>
@@ -1238,7 +1504,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>7</v>
+      </c>
+      <c r="R45">
+        <v>2</v>
+      </c>
       <c r="S45" t="s">
         <v>123</v>
       </c>
@@ -1249,7 +1521,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>8</v>
+      </c>
+      <c r="R46">
+        <v>4</v>
+      </c>
       <c r="S46" t="s">
         <v>74</v>
       </c>
@@ -1260,12 +1538,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="17:21" x14ac:dyDescent="0.25">
       <c r="T47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>9</v>
+      </c>
+      <c r="R48">
+        <v>2</v>
+      </c>
       <c r="S48" t="s">
         <v>91</v>
       </c>
@@ -1276,7 +1560,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>2</v>
+      </c>
+      <c r="R49">
+        <v>7</v>
+      </c>
       <c r="S49" t="s">
         <v>92</v>
       </c>
@@ -1287,7 +1577,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>3</v>
+      </c>
+      <c r="R50">
+        <v>9</v>
+      </c>
       <c r="S50" t="s">
         <v>93</v>
       </c>
@@ -1298,7 +1594,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <v>4</v>
+      </c>
+      <c r="R51">
+        <v>8</v>
+      </c>
       <c r="S51" t="s">
         <v>94</v>
       </c>
@@ -1309,7 +1611,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <v>10</v>
+      </c>
+      <c r="R52">
+        <v>3</v>
+      </c>
       <c r="S52" t="s">
         <v>95</v>
       </c>
@@ -1320,7 +1628,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>5</v>
+      </c>
+      <c r="R53">
+        <v>2</v>
+      </c>
       <c r="S53" t="s">
         <v>96</v>
       </c>
@@ -1331,7 +1645,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>10</v>
+      </c>
       <c r="S54" t="s">
         <v>97</v>
       </c>
@@ -1342,7 +1662,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <v>6</v>
+      </c>
+      <c r="R55">
+        <v>6</v>
+      </c>
       <c r="S55" t="s">
         <v>98</v>
       </c>
@@ -1353,7 +1679,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <v>5</v>
+      </c>
+      <c r="R56">
+        <v>7</v>
+      </c>
       <c r="S56" t="s">
         <v>99</v>
       </c>
@@ -1364,7 +1696,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q57">
+        <v>7</v>
+      </c>
+      <c r="R57">
+        <v>4</v>
+      </c>
       <c r="S57" t="s">
         <v>100</v>
       </c>
@@ -1375,7 +1713,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <v>8</v>
+      </c>
+      <c r="R58">
+        <v>5</v>
+      </c>
       <c r="S58" t="s">
         <v>101</v>
       </c>
@@ -1386,7 +1730,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <v>4</v>
+      </c>
+      <c r="R59">
+        <v>6</v>
+      </c>
       <c r="S59" t="s">
         <v>106</v>
       </c>
@@ -1397,7 +1747,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q60">
+        <v>3</v>
+      </c>
+      <c r="R60">
+        <v>9</v>
+      </c>
       <c r="S60" t="s">
         <v>102</v>
       </c>
@@ -1408,7 +1764,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <v>6</v>
+      </c>
+      <c r="R61">
+        <v>4</v>
+      </c>
       <c r="S61" t="s">
         <v>103</v>
       </c>
@@ -1419,7 +1781,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <v>7</v>
+      </c>
+      <c r="R62">
+        <v>5</v>
+      </c>
       <c r="S62" t="s">
         <v>104</v>
       </c>
@@ -1430,7 +1798,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <v>8</v>
+      </c>
+      <c r="R63">
+        <v>3</v>
+      </c>
       <c r="S63" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Working on Config Menu . . .
</commit_message>
<xml_diff>
--- a/Documantation/Final/Teams.xlsx
+++ b/Documantation/Final/Teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Project\Hamed Soleimani\Handy Football\Documantation\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC83FF31-E373-408B-8A03-CA7197E01913}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC70F5B-BBE5-4A1C-9916-1BE0574C4CA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5928" yWindow="480" windowWidth="11496" windowHeight="11304" xr2:uid="{ECF06A1F-CD2B-45BD-8D37-BFC9939645AD}"/>
   </bookViews>
@@ -756,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3753AAEB-6318-494D-9F15-E9F1EFFD60D3}">
   <dimension ref="P1:U63"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N42" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>

</xml_diff>